<commit_message>
calc acorr on sorted data
</commit_message>
<xml_diff>
--- a/acorr_tests.xlsx
+++ b/acorr_tests.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brazen\YandexDisk\ГУУ\3 курс\5 сем\Эконометрика\Курсовая работа\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4083928A-CA79-4DE1-8581-7F8ECA39ACD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6342876-28C3-45CB-88ED-64340D08B947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A99A8B2-AFFC-494D-81EF-8BC34ABF0C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,15 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>cluster_id</t>
-  </si>
-  <si>
-    <t>Статистики тестов</t>
-  </si>
-  <si>
-    <t>Порядок лага</t>
   </si>
   <si>
     <t>DW_L</t>
@@ -55,6 +50,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>\DW-stat</t>
+  </si>
+  <si>
+    <t>BG F-stat p-value</t>
   </si>
 </sst>
 </file>
@@ -86,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -217,16 +221,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -244,24 +365,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -271,21 +380,68 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -306,20 +462,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -333,7 +490,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -345,15 +502,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -367,7 +518,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -381,7 +532,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -395,86 +546,15 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -786,365 +866,817 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEF7454-2A5C-448B-B4BA-82944EB56253}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="16">
+        <v>0</v>
+      </c>
+      <c r="D1" s="17">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="17">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="17">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="17">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="H1" s="18">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="I1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>3</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1.24</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="F2" s="6">
+        <v>3.22</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3.18</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3.12</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.59</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2.77</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3.06</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3.24</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3.37</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1.41</v>
+      </c>
+      <c r="K3" s="5">
+        <v>2.59</v>
+      </c>
+      <c r="L3" s="5">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="14">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="C4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.01</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.54</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.57</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.42</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2.58</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.33</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3.22</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.18</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="L7" s="3">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.69</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.94</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3.36</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3.53</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.63</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.46</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2.54</v>
+      </c>
+      <c r="L9" s="3">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="35">
+        <v>0</v>
+      </c>
+      <c r="D12" s="23">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E12" s="23">
         <v>2</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F12" s="23">
         <v>3</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G12" s="23">
         <v>4</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H12" s="23">
         <v>5</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    </row>
+    <row r="13" spans="1:12" s="31" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="27">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="15">
+      <c r="B13" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="36">
         <v>0.59</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D13" s="28">
         <v>1.87</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E13" s="28">
         <v>2.77</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F13" s="28">
         <v>3.06</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G13" s="28">
         <v>3.24</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H13" s="28">
         <v>3.37</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I13" s="29">
         <v>0.88</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J13" s="30">
         <v>1.41</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K13" s="30">
         <v>2.59</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L13" s="30">
         <v>3.12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="E4" s="4">
+    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>1</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="26">
+        <v>0</v>
+      </c>
+      <c r="E14" s="26">
+        <v>0.26</v>
+      </c>
+      <c r="F14" s="26">
         <v>0.35</v>
       </c>
-      <c r="F4" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G14" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="H14" s="26">
         <v>0.15</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="I14" s="21"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
+        <v>1</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="23">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="16">
+      <c r="B16" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="38">
         <v>1.01</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D16" s="24">
         <v>1.35</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E16" s="24">
         <v>1.54</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F16" s="24">
         <v>1.57</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G16" s="24">
         <v>1.1499999999999999</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H16" s="24">
         <v>1.1499999999999999</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I16" s="22">
         <v>0.71</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J16" s="3">
         <v>1.42</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K16" s="3">
         <v>2.58</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L16" s="3">
         <v>3.29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4">
+    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="23">
+        <v>2</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0.89</v>
+      </c>
+      <c r="F17" s="24">
+        <v>0.44</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0.92</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0.93</v>
+      </c>
+      <c r="I17" s="22"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
+        <v>2</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="24">
         <v>0.08</v>
       </c>
-      <c r="E6" s="4">
-        <v>0.93</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.93</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="E18" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0.22</v>
+      </c>
+      <c r="G18" s="24">
+        <v>0.17</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="23">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="B19" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="38">
         <v>0.33</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D19" s="24">
         <v>1.24</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E19" s="24">
         <v>2.7</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F19" s="24">
         <v>3.22</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G19" s="24">
         <v>3.18</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H19" s="24">
         <v>3.12</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I19" s="22">
         <v>0.88</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J19" s="3">
         <v>1.41</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K19" s="3">
         <v>2.59</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L19" s="3">
         <v>3.12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.61</v>
-      </c>
-      <c r="G8" s="4">
+    <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="23">
+        <v>3</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="24">
         <v>0.71</v>
       </c>
-      <c r="H8" s="4">
+      <c r="G20" s="24">
+        <v>0.49</v>
+      </c>
+      <c r="H20" s="24">
         <v>0.17</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="I20" s="22"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="23">
+        <v>3</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0</v>
+      </c>
+      <c r="F21" s="24">
+        <v>0</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0</v>
+      </c>
+      <c r="H21" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="23">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B22" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="38">
         <v>0.38</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D22" s="24">
         <v>1.69</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E22" s="24">
         <v>2.94</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F22" s="24">
         <v>3.36</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G22" s="24">
         <v>3.53</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H22" s="24">
         <v>3.63</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I22" s="22">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J22" s="3">
         <v>1.46</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K22" s="3">
         <v>2.54</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L22" s="3">
         <v>2.85</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.36</v>
-      </c>
-      <c r="H10" s="4">
+    <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0.54</v>
+      </c>
+      <c r="G23" s="24">
+        <v>0.43</v>
+      </c>
+      <c r="H23" s="24">
         <v>0.67</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="23">
+        <v>4</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="38"/>
+      <c r="D24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="24">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="4">
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:H5 C7:H7 C9:H9 C3:H3">
-    <cfRule type="expression" dxfId="9" priority="6">
-      <formula>C3&lt;$I3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
-      <formula>OR( AND($I3&lt;C3,C3&lt;$J3), AND($K3 &lt; C3,C3 &lt;$L3))</formula>
+  <conditionalFormatting sqref="D14:H15 D17:H18 D20:H21 D23:H24">
+    <cfRule type="expression" dxfId="16" priority="1">
+      <formula>D14 &lt;= 0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:H3 C5:H5 C7:H7 C9:H9">
-    <cfRule type="expression" dxfId="7" priority="4">
-      <formula>C3&gt;=$L3</formula>
+  <conditionalFormatting sqref="C16:H16">
+    <cfRule type="expression" dxfId="15" priority="7">
+      <formula>AND($J17&lt; C16,C16 &lt; $K17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="8">
+      <formula>C16&gt;=$L17</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="9">
+      <formula>OR( AND($I17&lt;C16,C16&lt;$J17), AND($K17 &lt; C16,C16 &lt;$L17))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>C16&lt;$I17</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:H3 C5 C5:H5 C7:H7 C9:H9">
-    <cfRule type="expression" dxfId="6" priority="3">
-      <formula>AND($J3&lt; C3,C3 &lt; $K3)</formula>
+  <conditionalFormatting sqref="C22:H22">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>AND(#REF!&lt; C22,C22 &lt; #REF!)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>C22&gt;=#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="13">
+      <formula>OR( AND(#REF!&lt;C22,C22&lt;#REF!), AND(#REF! &lt; C22,C22 &lt;#REF!))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="14">
+      <formula>C22&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:H4 C6:H6 C8:H8 C10:H10">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>C4 &lt;= 0.05</formula>
+  <conditionalFormatting sqref="C19:H19">
+    <cfRule type="expression" dxfId="7" priority="19">
+      <formula>AND($J22&lt; C19,C19 &lt; $K22)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="20">
+      <formula>C19&gt;=$L22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="21">
+      <formula>OR( AND($I22&lt;C19,C19&lt;$J22), AND($K22 &lt; C19,C19 &lt;$L22))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="22">
+      <formula>C19&lt;$I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:H13 C16:H16 C19:H19 C22:H22">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>AND($J13&lt; C13,C13 &lt; $K13)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>OR( AND($I13&lt;C13,C13&lt;$J13), AND($K13 &lt; C13,C13 &lt;$L13))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>C13&lt;$I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:H16 C13:H13 C19:H19 C22:H22">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>C13&gt;=$L13</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5D1C2E-9529-49DF-BD5C-987376C22D19}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added coef restriction a + b = 1
</commit_message>
<xml_diff>
--- a/acorr_tests.xlsx
+++ b/acorr_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brazen\YandexDisk\ГУУ\3 курс\5 сем\Эконометрика\Курсовая работа\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638BBDD5-E8C1-4A67-A2C9-86A4C6416032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60007E6F-531D-4775-B3DF-2580D32BC249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4A99A8B2-AFFC-494D-81EF-8BC34ABF0C64}"/>
   </bookViews>
@@ -377,7 +377,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="26">
     <dxf>
       <font>
         <b/>
@@ -547,226 +547,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1564,7 +1344,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,8 +1352,7 @@
     <col min="1" max="1" width="11.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
@@ -1634,43 +1413,43 @@
         <v>1</v>
       </c>
       <c r="C2" s="26">
-        <v>2.75</v>
+        <v>0.59</v>
       </c>
       <c r="D2" s="27">
-        <v>2.2200000000000002</v>
+        <v>1.87</v>
       </c>
       <c r="E2" s="27">
-        <v>1.84</v>
+        <v>2.77</v>
       </c>
       <c r="F2" s="27">
-        <v>1.5</v>
+        <v>3.06</v>
       </c>
       <c r="G2" s="27">
-        <v>1.19</v>
+        <v>3.24</v>
       </c>
       <c r="H2" s="27">
-        <v>0.93</v>
+        <v>3.37</v>
       </c>
       <c r="I2" s="27">
-        <v>0.74</v>
+        <v>3.46</v>
       </c>
       <c r="J2" s="27">
-        <v>0.62</v>
+        <v>3.52</v>
       </c>
       <c r="K2" s="27">
-        <v>0.54</v>
+        <v>3.55</v>
       </c>
       <c r="L2" s="27">
-        <v>0.49</v>
+        <v>3.57</v>
       </c>
       <c r="M2" s="27">
-        <v>0.45</v>
+        <v>3.58</v>
       </c>
       <c r="N2" s="27">
-        <v>0.42</v>
+        <v>3.59</v>
       </c>
       <c r="O2" s="27">
-        <v>0.41</v>
+        <v>3.59</v>
       </c>
       <c r="T2" s="11">
         <v>0.88</v>
@@ -1694,40 +1473,40 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="30">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E3" s="30">
         <v>0.26</v>
       </c>
       <c r="F3" s="30">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="G3" s="30">
-        <v>0.49</v>
+        <v>0.12</v>
       </c>
       <c r="H3" s="30">
-        <v>0.28999999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="I3" s="30">
-        <v>0.31</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J3" s="30">
-        <v>0.27</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K3" s="30">
-        <v>0.24</v>
+        <v>0.36</v>
       </c>
       <c r="L3" s="30">
-        <v>0.37</v>
+        <v>0.32</v>
       </c>
       <c r="M3" s="30">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="N3" s="30">
-        <v>0.04</v>
+        <v>0.8</v>
       </c>
       <c r="O3" s="30">
-        <v>0.37</v>
+        <v>0.69</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="2"/>
@@ -1743,40 +1522,40 @@
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="32">
+        <v>0</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="I4" s="32">
         <v>0.03</v>
       </c>
-      <c r="E4" s="32">
-        <v>0.09</v>
-      </c>
-      <c r="F4" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="G4" s="32">
-        <v>0.12</v>
-      </c>
-      <c r="H4" s="32">
-        <v>0.18</v>
-      </c>
-      <c r="I4" s="32">
-        <v>0.27</v>
-      </c>
       <c r="J4" s="32">
-        <v>0.35</v>
+        <v>0.06</v>
       </c>
       <c r="K4" s="32">
-        <v>0.42</v>
+        <v>0.11</v>
       </c>
       <c r="L4" s="32">
-        <v>0.54</v>
+        <v>0.17</v>
       </c>
       <c r="M4" s="32">
-        <v>0.55000000000000004</v>
+        <v>0.24</v>
       </c>
       <c r="N4" s="32">
-        <v>0.31</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="O4" s="32">
-        <v>0.42</v>
+        <v>0.38</v>
       </c>
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
@@ -1791,43 +1570,43 @@
         <v>1</v>
       </c>
       <c r="C5" s="31">
-        <v>2.17</v>
+        <v>1.01</v>
       </c>
       <c r="D5" s="32">
-        <v>2.1800000000000002</v>
+        <v>1.35</v>
       </c>
       <c r="E5" s="32">
-        <v>2.2000000000000002</v>
+        <v>1.54</v>
       </c>
       <c r="F5" s="32">
-        <v>2.21</v>
+        <v>1.57</v>
       </c>
       <c r="G5" s="32">
-        <v>2.2000000000000002</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H5" s="32">
-        <v>2.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="I5" s="32">
-        <v>2.12</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="J5" s="32">
-        <v>2.04</v>
+        <v>2.68</v>
       </c>
       <c r="K5" s="32">
-        <v>1.94</v>
+        <v>2.91</v>
       </c>
       <c r="L5" s="32">
-        <v>1.82</v>
+        <v>3.01</v>
       </c>
       <c r="M5" s="32">
-        <v>1.69</v>
+        <v>3.11</v>
       </c>
       <c r="N5" s="32">
-        <v>1.55</v>
+        <v>3.21</v>
       </c>
       <c r="O5" s="32">
-        <v>1.41</v>
+        <v>3.29</v>
       </c>
       <c r="T5" s="4">
         <v>0.71</v>
@@ -1851,40 +1630,40 @@
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="32">
-        <v>0.3</v>
+        <v>0.04</v>
       </c>
       <c r="E6" s="32">
-        <v>0.02</v>
+        <v>0.89</v>
       </c>
       <c r="F6" s="32">
-        <v>0.49</v>
+        <v>0.44</v>
       </c>
       <c r="G6" s="32">
-        <v>0.01</v>
+        <v>0.92</v>
       </c>
       <c r="H6" s="32">
-        <v>0.14000000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="I6" s="32">
-        <v>0.37</v>
+        <v>0.87</v>
       </c>
       <c r="J6" s="32">
-        <v>0.22</v>
+        <v>0.98</v>
       </c>
       <c r="K6" s="32">
-        <v>0.28000000000000003</v>
+        <v>0.75</v>
       </c>
       <c r="L6" s="32">
-        <v>0.46</v>
+        <v>0.97</v>
       </c>
       <c r="M6" s="32">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="N6" s="32">
-        <v>0.3</v>
+        <v>0.92</v>
       </c>
       <c r="O6" s="32">
-        <v>0.39</v>
+        <v>0.84</v>
       </c>
       <c r="T6" s="4"/>
       <c r="U6" s="1"/>
@@ -1900,40 +1679,40 @@
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="32">
-        <v>0.6</v>
+        <v>0.08</v>
       </c>
       <c r="E7" s="32">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F7" s="32">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="G7" s="32">
+        <v>0.17</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0.13</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0.03</v>
+      </c>
+      <c r="K7" s="32">
+        <v>0.06</v>
+      </c>
+      <c r="L7" s="32">
+        <v>0.03</v>
+      </c>
+      <c r="M7" s="32">
         <v>0.02</v>
       </c>
-      <c r="H7" s="32">
-        <v>0.04</v>
-      </c>
-      <c r="I7" s="32">
-        <v>0.08</v>
-      </c>
-      <c r="J7" s="32">
-        <v>0.12</v>
-      </c>
-      <c r="K7" s="32">
-        <v>0.19</v>
-      </c>
-      <c r="L7" s="32">
-        <v>0.33</v>
-      </c>
-      <c r="M7" s="32">
-        <v>0.5</v>
-      </c>
       <c r="N7" s="32">
-        <v>0.63</v>
+        <v>0.02</v>
       </c>
       <c r="O7" s="32">
-        <v>0.79</v>
+        <v>0.05</v>
       </c>
       <c r="T7" s="24"/>
       <c r="U7" s="24"/>
@@ -1948,43 +1727,43 @@
         <v>1</v>
       </c>
       <c r="C8" s="31">
-        <v>2.6</v>
+        <v>0.33</v>
       </c>
       <c r="D8" s="32">
-        <v>2.2200000000000002</v>
+        <v>1.24</v>
       </c>
       <c r="E8" s="32">
-        <v>1.94</v>
+        <v>2.7</v>
       </c>
       <c r="F8" s="32">
-        <v>1.7</v>
+        <v>3.22</v>
       </c>
       <c r="G8" s="32">
-        <v>1.46</v>
+        <v>3.18</v>
       </c>
       <c r="H8" s="32">
-        <v>1.24</v>
+        <v>3.12</v>
       </c>
       <c r="I8" s="32">
-        <v>1.07</v>
+        <v>3.1</v>
       </c>
       <c r="J8" s="32">
-        <v>0.94</v>
+        <v>3.14</v>
       </c>
       <c r="K8" s="32">
-        <v>0.84</v>
+        <v>3.23</v>
       </c>
       <c r="L8" s="32">
-        <v>0.77</v>
+        <v>3.31</v>
       </c>
       <c r="M8" s="32">
-        <v>0.71</v>
+        <v>3.35</v>
       </c>
       <c r="N8" s="32">
-        <v>0.67</v>
+        <v>3.35</v>
       </c>
       <c r="O8" s="32">
-        <v>0.64</v>
+        <v>3.33</v>
       </c>
       <c r="T8" s="4">
         <v>0.88</v>
@@ -2008,40 +1787,40 @@
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="32">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E9" s="32">
-        <v>0.04</v>
+        <v>0.8</v>
       </c>
       <c r="F9" s="32">
+        <v>0.71</v>
+      </c>
+      <c r="G9" s="32">
+        <v>0.49</v>
+      </c>
+      <c r="H9" s="32">
         <v>0.17</v>
       </c>
-      <c r="G9" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="H9" s="32">
-        <v>0.4</v>
-      </c>
       <c r="I9" s="32">
-        <v>0.26</v>
+        <v>0.06</v>
       </c>
       <c r="J9" s="32">
-        <v>0.16</v>
+        <v>0.37</v>
       </c>
       <c r="K9" s="32">
-        <v>0.14000000000000001</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="L9" s="32">
-        <v>0.32</v>
+        <v>0.45</v>
       </c>
       <c r="M9" s="32">
-        <v>0.23</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="N9" s="32">
-        <v>7.0000000000000007E-2</v>
+        <v>0.6</v>
       </c>
       <c r="O9" s="32">
-        <v>0.46</v>
+        <v>0.91</v>
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="1"/>
@@ -2057,40 +1836,40 @@
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10" s="32">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0</v>
+      </c>
+      <c r="G10" s="32">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0</v>
+      </c>
+      <c r="J10" s="32">
+        <v>0</v>
+      </c>
+      <c r="K10" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="L10" s="32">
+        <v>0.03</v>
+      </c>
+      <c r="M10" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="N10" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="O10" s="32">
         <v>0.08</v>
-      </c>
-      <c r="E10" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="F10" s="32">
-        <v>0.08</v>
-      </c>
-      <c r="G10" s="32">
-        <v>0.15</v>
-      </c>
-      <c r="H10" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="I10" s="32">
-        <v>0.33</v>
-      </c>
-      <c r="J10" s="32">
-        <v>0.35</v>
-      </c>
-      <c r="K10" s="32">
-        <v>0.33</v>
-      </c>
-      <c r="L10" s="32">
-        <v>0.43</v>
-      </c>
-      <c r="M10" s="32">
-        <v>0.49</v>
-      </c>
-      <c r="N10" s="32">
-        <v>0.35</v>
-      </c>
-      <c r="O10" s="32">
-        <v>0.48</v>
       </c>
       <c r="T10" s="24"/>
       <c r="U10" s="24"/>
@@ -2105,43 +1884,43 @@
         <v>1</v>
       </c>
       <c r="C11" s="31">
-        <v>2.37</v>
+        <v>0.38</v>
       </c>
       <c r="D11" s="32">
-        <v>2.12</v>
+        <v>1.69</v>
       </c>
       <c r="E11" s="32">
-        <v>1.92</v>
+        <v>2.94</v>
       </c>
       <c r="F11" s="32">
-        <v>1.76</v>
+        <v>3.36</v>
       </c>
       <c r="G11" s="32">
-        <v>1.61</v>
+        <v>3.53</v>
       </c>
       <c r="H11" s="32">
-        <v>1.43</v>
+        <v>3.63</v>
       </c>
       <c r="I11" s="32">
-        <v>1.23</v>
+        <v>3.7</v>
       </c>
       <c r="J11" s="32">
-        <v>1.03</v>
+        <v>3.74</v>
       </c>
       <c r="K11" s="32">
-        <v>0.83</v>
+        <v>3.77</v>
       </c>
       <c r="L11" s="32">
-        <v>0.67</v>
+        <v>3.8</v>
       </c>
       <c r="M11" s="32">
-        <v>0.54</v>
+        <v>3.81</v>
       </c>
       <c r="N11" s="32">
-        <v>0.44</v>
+        <v>3.83</v>
       </c>
       <c r="O11" s="32">
-        <v>0.36</v>
+        <v>3.84</v>
       </c>
       <c r="T11" s="4">
         <v>1.1499999999999999</v>
@@ -2165,40 +1944,40 @@
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="32">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="E12" s="32">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="F12" s="32">
-        <v>0.22</v>
+        <v>0.54</v>
       </c>
       <c r="G12" s="32">
-        <v>0.28000000000000003</v>
+        <v>0.43</v>
       </c>
       <c r="H12" s="32">
-        <v>0.28999999999999998</v>
+        <v>0.67</v>
       </c>
       <c r="I12" s="32">
-        <v>0.18</v>
+        <v>0.42</v>
       </c>
       <c r="J12" s="32">
-        <v>0.13</v>
+        <v>0.42</v>
       </c>
       <c r="K12" s="32">
-        <v>0.14000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="L12" s="32">
-        <v>0.2</v>
+        <v>0.41</v>
       </c>
       <c r="M12" s="32">
-        <v>0.41</v>
+        <v>0.53</v>
       </c>
       <c r="N12" s="32">
-        <v>0.49</v>
+        <v>0.74</v>
       </c>
       <c r="O12" s="32">
-        <v>0.35</v>
+        <v>0.88</v>
       </c>
       <c r="T12" s="4"/>
       <c r="U12" s="1"/>
@@ -2214,40 +1993,40 @@
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="32">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="E13" s="32">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="F13" s="32">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="G13" s="32">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="32">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="I13" s="32">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J13" s="32">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K13" s="32">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="L13" s="32">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="M13" s="32">
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="N13" s="32">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="O13" s="32">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="T13" s="24"/>
       <c r="U13" s="24"/>

</xml_diff>